<commit_message>
fixes toma de std
</commit_message>
<xml_diff>
--- a/memoria/pasillo/pasillo.xlsx
+++ b/memoria/pasillo/pasillo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diazu\MT-MARL\memoria\pasillo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5367C8E9-7BE2-4FAB-9315-2218F5ED9F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BA2C38-2077-4AA0-AFFF-EE09AA3F2C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="28155" windowHeight="14490" xr2:uid="{77BDEF68-C8AA-4190-91B4-454775195A81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77BDEF68-C8AA-4190-91B4-454775195A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="31">
-  <si>
-    <t>costo_por_agente</t>
-  </si>
-  <si>
-    <t>completion_time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="32">
   <si>
     <t>valores_ideales</t>
   </si>
@@ -64,9 +58,6 @@
   </si>
   <si>
     <t>STDEV</t>
-  </si>
-  <si>
-    <t>tiempo_en_acabar (success_agents)</t>
   </si>
   <si>
     <t>agentes_en_goal</t>
@@ -127,6 +118,18 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>sum_of_costs</t>
+  </si>
+  <si>
+    <t>makespan</t>
+  </si>
+  <si>
+    <t>completion_time</t>
+  </si>
+  <si>
+    <t>tiempo_en_acabar</t>
   </si>
 </sst>
 </file>
@@ -220,11 +223,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-CL" baseline="0"/>
-              <a:t> c</a:t>
+              <a:t> sum of costs </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-CL"/>
-              <a:t>osto desplazamiento MARL</a:t>
+              <a:t>MARL</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-CL" baseline="0"/>
@@ -1393,7 +1396,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-CL"/>
-              <a:t>Avg costo tiempo</a:t>
+              <a:t>Avg makespan</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-CL" baseline="0"/>
@@ -1810,61 +1813,61 @@
                     <c:v>23.327751177513871</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.034063544529189</c:v>
+                    <c:v>16.02309271021047</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.71761789453857</c:v>
+                    <c:v>10.70626345105207</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3362659737430462</c:v>
+                    <c:v>7.3338399890081467</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0081926343387559</c:v>
+                    <c:v>7.018378997318397</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.2325759972194934</c:v>
+                    <c:v>7.244915075033278</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6.3314820781648313</c:v>
+                    <c:v>6.3562188333271594</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>8.0349354141383742</c:v>
+                    <c:v>8.0548149177603712</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>5.6262996852414604</c:v>
+                    <c:v>5.6637104489356371</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>4.2580088950118453</c:v>
+                    <c:v>4.36699450423286</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>61.631361220556869</c:v>
+                    <c:v>89.758543183254503</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>47.707516255284823</c:v>
+                    <c:v>64.068736977895142</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>61.004841698130043</c:v>
+                    <c:v>85.313685592472808</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>59.184305372484268</c:v>
+                    <c:v>79.898867349885776</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>39.613582092790118</c:v>
+                    <c:v>68.829472014174272</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>98.055387793292468</c:v>
+                    <c:v>132.7864576232268</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>33.684412984556907</c:v>
+                    <c:v>48.167479372680972</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>52.110211433354003</c:v>
+                    <c:v>89.944275228784448</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>47.154079611741658</c:v>
+                    <c:v>80.988743446726218</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>72.080161108895794</c:v>
+                    <c:v>106.36452961036581</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1879,61 +1882,61 @@
                     <c:v>23.327751177513871</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.034063544529189</c:v>
+                    <c:v>16.02309271021047</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.71761789453857</c:v>
+                    <c:v>10.70626345105207</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3362659737430462</c:v>
+                    <c:v>7.3338399890081467</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0081926343387559</c:v>
+                    <c:v>7.018378997318397</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.2325759972194934</c:v>
+                    <c:v>7.244915075033278</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6.3314820781648313</c:v>
+                    <c:v>6.3562188333271594</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>8.0349354141383742</c:v>
+                    <c:v>8.0548149177603712</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>5.6262996852414604</c:v>
+                    <c:v>5.6637104489356371</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>4.2580088950118453</c:v>
+                    <c:v>4.36699450423286</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>61.631361220556869</c:v>
+                    <c:v>89.758543183254503</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>47.707516255284823</c:v>
+                    <c:v>64.068736977895142</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>61.004841698130043</c:v>
+                    <c:v>85.313685592472808</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>59.184305372484268</c:v>
+                    <c:v>79.898867349885776</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>39.613582092790118</c:v>
+                    <c:v>68.829472014174272</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>98.055387793292468</c:v>
+                    <c:v>132.7864576232268</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>33.684412984556907</c:v>
+                    <c:v>48.167479372680972</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>52.110211433354003</c:v>
+                    <c:v>89.944275228784448</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>47.154079611741658</c:v>
+                    <c:v>80.988743446726218</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>72.080161108895794</c:v>
+                    <c:v>106.36452961036581</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2105,7 +2108,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>completion_time</c:v>
+                  <c:v>makespan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9262,8 +9265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B691F5-4794-4A6A-A54B-EFD8B65B6485}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V59" sqref="V59"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9274,47 +9277,47 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
         <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>30.835000000000001</v>
@@ -9332,7 +9335,7 @@
         <v>30.2</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>91.655000000000001</v>
@@ -9352,7 +9355,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>24.13</v>
@@ -9370,7 +9373,7 @@
         <v>23.2</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I4">
         <v>70.032499999999999</v>
@@ -9382,7 +9385,7 @@
         <v>71.075000000000003</v>
       </c>
       <c r="L4">
-        <v>16.034063544529189</v>
+        <v>16.02309271021047</v>
       </c>
       <c r="M4">
         <v>23.2</v>
@@ -9390,7 +9393,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>29.875</v>
@@ -9408,7 +9411,7 @@
         <v>23.8</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I5">
         <v>71.2</v>
@@ -9420,7 +9423,7 @@
         <v>72.335833333333341</v>
       </c>
       <c r="L5">
-        <v>10.71761789453857</v>
+        <v>10.70626345105207</v>
       </c>
       <c r="M5">
         <v>23.8</v>
@@ -9428,7 +9431,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>30.591249999999999</v>
@@ -9446,7 +9449,7 @@
         <v>20.675000000000001</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I6">
         <v>88.408749999999998</v>
@@ -9458,7 +9461,7 @@
         <v>89.434375000000003</v>
       </c>
       <c r="L6">
-        <v>7.3362659737430462</v>
+        <v>7.3338399890081467</v>
       </c>
       <c r="M6">
         <v>20.675000000000001</v>
@@ -9466,7 +9469,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>31.91</v>
@@ -9484,7 +9487,7 @@
         <v>22.3</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>60.405999999999992</v>
@@ -9496,7 +9499,7 @@
         <v>61.522500000000001</v>
       </c>
       <c r="L7">
-        <v>7.0081926343387559</v>
+        <v>7.018378997318397</v>
       </c>
       <c r="M7">
         <v>22.3</v>
@@ -9504,7 +9507,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>26.619166666666661</v>
@@ -9522,7 +9525,7 @@
         <v>21.366666666666671</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>53.75333333333333</v>
@@ -9534,7 +9537,7 @@
         <v>54.83</v>
       </c>
       <c r="L8">
-        <v>7.2325759972194934</v>
+        <v>7.244915075033278</v>
       </c>
       <c r="M8">
         <v>21.366666666666671</v>
@@ -9542,7 +9545,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>57.341428571428573</v>
@@ -9560,7 +9563,7 @@
         <v>23.714285714285719</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I9">
         <v>82.76</v>
@@ -9572,7 +9575,7 @@
         <v>84.139285714285705</v>
       </c>
       <c r="L9">
-        <v>6.3314820781648313</v>
+        <v>6.3562188333271594</v>
       </c>
       <c r="M9">
         <v>23.714285714285719</v>
@@ -9580,7 +9583,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>65.791875000000005</v>
@@ -9598,7 +9601,7 @@
         <v>25.087499999999999</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I10">
         <v>101.674375</v>
@@ -9610,7 +9613,7 @@
         <v>103.076875</v>
       </c>
       <c r="L10">
-        <v>8.0349354141383742</v>
+        <v>8.0548149177603712</v>
       </c>
       <c r="M10">
         <v>25.087499999999999</v>
@@ -9618,7 +9621,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>67.290000000000006</v>
@@ -9636,7 +9639,7 @@
         <v>23.62222222222222</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I11">
         <v>89.603333333333325</v>
@@ -9648,7 +9651,7 @@
         <v>91.162222222222226</v>
       </c>
       <c r="L11">
-        <v>5.6262996852414604</v>
+        <v>5.6637104489356371</v>
       </c>
       <c r="M11">
         <v>23.62222222222222</v>
@@ -9656,7 +9659,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>70.353999999999999</v>
@@ -9674,7 +9677,7 @@
         <v>24.73</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <v>76.300500000000014</v>
@@ -9686,7 +9689,7 @@
         <v>77.968000000000004</v>
       </c>
       <c r="L12">
-        <v>4.2580088950118453</v>
+        <v>4.36699450423286</v>
       </c>
       <c r="M12">
         <v>24.73</v>
@@ -9694,7 +9697,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>66.369090909090914</v>
@@ -9712,7 +9715,7 @@
         <v>24.618181818181821</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I13">
         <v>106.0206818181818</v>
@@ -9724,7 +9727,7 @@
         <v>116.1409090909091</v>
       </c>
       <c r="L13">
-        <v>61.631361220556869</v>
+        <v>89.758543183254503</v>
       </c>
       <c r="M13">
         <v>24.618181818181821</v>
@@ -9732,7 +9735,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>82.610416666666666</v>
@@ -9750,7 +9753,7 @@
         <v>24.583333333333329</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>105.92020833333331</v>
@@ -9762,7 +9765,7 @@
         <v>110.371875</v>
       </c>
       <c r="L14">
-        <v>47.707516255284823</v>
+        <v>64.068736977895142</v>
       </c>
       <c r="M14">
         <v>24.583333333333329</v>
@@ -9770,7 +9773,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>106.0857692307693</v>
@@ -9788,7 +9791,7 @@
         <v>24.838461538461541</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I15">
         <v>127.4221153846154</v>
@@ -9800,7 +9803,7 @@
         <v>135.62442307692311</v>
       </c>
       <c r="L15">
-        <v>61.004841698130043</v>
+        <v>85.313685592472808</v>
       </c>
       <c r="M15">
         <v>24.838461538461541</v>
@@ -9808,7 +9811,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>90.408928571428575</v>
@@ -9826,7 +9829,7 @@
         <v>24.25714285714286</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I16">
         <v>108.52892857142859</v>
@@ -9838,7 +9841,7 @@
         <v>116.47125</v>
       </c>
       <c r="L16">
-        <v>59.184305372484268</v>
+        <v>79.898867349885776</v>
       </c>
       <c r="M16">
         <v>24.25714285714286</v>
@@ -9846,7 +9849,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17">
         <v>91.795000000000002</v>
@@ -9864,7 +9867,7 @@
         <v>23.32</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I17">
         <v>95.617333333333335</v>
@@ -9876,7 +9879,7 @@
         <v>104.2848333333333</v>
       </c>
       <c r="L17">
-        <v>39.613582092790118</v>
+        <v>68.829472014174272</v>
       </c>
       <c r="M17">
         <v>23.32</v>
@@ -9884,7 +9887,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>160.11296874999999</v>
@@ -9902,7 +9905,7 @@
         <v>26.675000000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I18">
         <v>157.69593750000001</v>
@@ -9914,7 +9917,7 @@
         <v>172.82499999999999</v>
       </c>
       <c r="L18">
-        <v>98.055387793292468</v>
+        <v>132.7864576232268</v>
       </c>
       <c r="M18">
         <v>26.675000000000001</v>
@@ -9922,7 +9925,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>120.7623529411765</v>
@@ -9940,7 +9943,7 @@
         <v>23.764705882352938</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I19">
         <v>99.985588235294117</v>
@@ -9952,7 +9955,7 @@
         <v>105.8326470588235</v>
       </c>
       <c r="L19">
-        <v>33.684412984556907</v>
+        <v>48.167479372680972</v>
       </c>
       <c r="M19">
         <v>23.764705882352938</v>
@@ -9960,7 +9963,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>137.25416666666669</v>
@@ -9978,7 +9981,7 @@
         <v>23.977777777777781</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I20">
         <v>120.8879166666667</v>
@@ -9990,7 +9993,7 @@
         <v>136.57458333333341</v>
       </c>
       <c r="L20">
-        <v>52.110211433354003</v>
+        <v>89.944275228784448</v>
       </c>
       <c r="M20">
         <v>23.977777777777781</v>
@@ -9998,7 +10001,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>143.82526315789471</v>
@@ -10016,7 +10019,7 @@
         <v>24.147368421052629</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I21">
         <v>115.38552631578951</v>
@@ -10028,7 +10031,7 @@
         <v>127.7669736842105</v>
       </c>
       <c r="L21">
-        <v>47.154079611741658</v>
+        <v>80.988743446726218</v>
       </c>
       <c r="M21">
         <v>24.147368421052629</v>
@@ -10036,7 +10039,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>107.52800000000001</v>
@@ -10054,7 +10057,7 @@
         <v>22.6</v>
       </c>
       <c r="H22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I22">
         <v>122.51537500000001</v>
@@ -10066,7 +10069,7 @@
         <v>139.33837500000001</v>
       </c>
       <c r="L22">
-        <v>72.080161108895794</v>
+        <v>106.36452961036581</v>
       </c>
       <c r="M22">
         <v>22.6</v>
@@ -10074,27 +10077,27 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
       <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
         <v>7</v>
-      </c>
-      <c r="H26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B27">
         <v>48</v>
@@ -10106,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G27">
         <v>335.15</v>
@@ -10120,7 +10123,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>50.9</v>
@@ -10132,7 +10135,7 @@
         <v>5.3722935941307801</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G28">
         <v>489.9</v>
@@ -10146,7 +10149,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>78.375</v>
@@ -10158,7 +10161,7 @@
         <v>13.951725378090018</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G29">
         <v>439.6</v>
@@ -10172,7 +10175,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>118.52500000000001</v>
@@ -10184,7 +10187,7 @@
         <v>30.123666051964122</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <v>506.95</v>
@@ -10198,7 +10201,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>121.4</v>
@@ -10210,7 +10213,7 @@
         <v>24.370852704377434</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>437.4</v>
@@ -10224,7 +10227,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B32">
         <v>100.575</v>
@@ -10236,7 +10239,7 @@
         <v>19.710582215704637</v>
       </c>
       <c r="F32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G32">
         <v>545.25</v>
@@ -10250,7 +10253,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>275.35000000000002</v>
@@ -10262,7 +10265,7 @@
         <v>55.236809540424495</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G33">
         <v>544.9</v>
@@ -10276,7 +10279,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>318.45</v>
@@ -10288,7 +10291,7 @@
         <v>52.229743957309914</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G34">
         <v>571.67499999999995</v>
@@ -10302,7 +10305,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B35">
         <v>334.52499999999998</v>
@@ -10314,7 +10317,7 @@
         <v>48.453513275282106</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G35">
         <v>601.25</v>
@@ -10328,7 +10331,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B36">
         <v>344.17500000000001</v>
@@ -10340,7 +10343,7 @@
         <v>60.361257527129268</v>
       </c>
       <c r="F36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G36">
         <v>590.9</v>
@@ -10354,7 +10357,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B37">
         <v>346.22500000000002</v>
@@ -10366,7 +10369,7 @@
         <v>53.134318187314307</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>558.25</v>
@@ -10380,7 +10383,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <v>416.625</v>
@@ -10392,7 +10395,7 @@
         <v>56.677987179938128</v>
       </c>
       <c r="F38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G38">
         <v>588.17499999999995</v>
@@ -10406,7 +10409,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B39">
         <v>507.55</v>
@@ -10418,7 +10421,7 @@
         <v>70.053807158754097</v>
       </c>
       <c r="F39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G39">
         <v>567.875</v>
@@ -10432,7 +10435,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B40">
         <v>496.2</v>
@@ -10444,7 +10447,7 @@
         <v>72.11038546775147</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G40">
         <v>564.65</v>
@@ -10458,7 +10461,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B41">
         <v>503.75</v>
@@ -10470,7 +10473,7 @@
         <v>66.852976843372602</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G41">
         <v>619.85</v>
@@ -10484,7 +10487,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>721.65</v>
@@ -10496,7 +10499,7 @@
         <v>85.44290341268713</v>
       </c>
       <c r="F42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G42">
         <v>581.22500000000002</v>
@@ -10510,7 +10513,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B43">
         <v>644.27499999999998</v>
@@ -10522,7 +10525,7 @@
         <v>72.837010703385673</v>
       </c>
       <c r="F43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>621.07500000000005</v>
@@ -10536,7 +10539,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B44">
         <v>718.97500000000002</v>
@@ -10548,7 +10551,7 @@
         <v>105.3306119820485</v>
       </c>
       <c r="F44" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G44">
         <v>604.54999999999995</v>
@@ -10562,7 +10565,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B45">
         <v>761.95</v>
@@ -10574,7 +10577,7 @@
         <v>113.16970465315359</v>
       </c>
       <c r="F45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G45">
         <v>650.27499999999998</v>
@@ -10588,7 +10591,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46">
         <v>626.17499999999995</v>
@@ -10600,7 +10603,7 @@
         <v>65.487085240781198</v>
       </c>
       <c r="F46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G46">
         <v>590.5</v>
@@ -10614,27 +10617,27 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="H50" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B51">
         <v>48</v>
@@ -10646,7 +10649,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G51">
         <v>335.15</v>
@@ -10660,7 +10663,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>50.9</v>
@@ -10672,7 +10675,7 @@
         <v>5.3722935941307801</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G52">
         <v>489.9</v>
@@ -10686,7 +10689,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B53">
         <v>78.375</v>
@@ -10698,7 +10701,7 @@
         <v>13.951725378090018</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G53">
         <v>439.6</v>
@@ -10712,7 +10715,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>118.52500000000001</v>
@@ -10724,7 +10727,7 @@
         <v>30.123666051964122</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G54">
         <v>506.95</v>
@@ -10738,7 +10741,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B55">
         <v>121.4</v>
@@ -10750,7 +10753,7 @@
         <v>24.370852704377434</v>
       </c>
       <c r="F55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>437.4</v>
@@ -10764,7 +10767,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B56">
         <v>100.575</v>
@@ -10776,7 +10779,7 @@
         <v>19.710582215704637</v>
       </c>
       <c r="F56" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G56">
         <v>545.25</v>
@@ -10790,7 +10793,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B57">
         <v>275.35000000000002</v>
@@ -10802,7 +10805,7 @@
         <v>55.236809540424495</v>
       </c>
       <c r="F57" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G57">
         <v>544.9</v>
@@ -10816,7 +10819,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58">
         <v>318.45</v>
@@ -10828,7 +10831,7 @@
         <v>52.229743957309914</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G58">
         <v>571.67499999999995</v>
@@ -10842,7 +10845,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B59">
         <v>334.52499999999998</v>
@@ -10854,7 +10857,7 @@
         <v>48.453513275282106</v>
       </c>
       <c r="F59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G59">
         <v>601.25</v>
@@ -10868,7 +10871,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B60">
         <v>344.17500000000001</v>
@@ -10880,7 +10883,7 @@
         <v>60.361257527129268</v>
       </c>
       <c r="F60" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G60">
         <v>590.9</v>
@@ -10894,7 +10897,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B61">
         <v>346.22500000000002</v>
@@ -10906,7 +10909,7 @@
         <v>53.134318187314307</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G61">
         <v>629.54999999999995</v>
@@ -10920,7 +10923,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B62">
         <v>416.625</v>
@@ -10932,7 +10935,7 @@
         <v>56.677987179938128</v>
       </c>
       <c r="F62" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G62">
         <v>612.02499999999998</v>
@@ -10946,7 +10949,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B63">
         <v>507.55</v>
@@ -10958,7 +10961,7 @@
         <v>70.053807158754097</v>
       </c>
       <c r="F63" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G63">
         <v>614.6</v>
@@ -10972,7 +10975,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B64">
         <v>496.2</v>
@@ -10984,7 +10987,7 @@
         <v>72.11038546775147</v>
       </c>
       <c r="F64" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G64">
         <v>635.375</v>
@@ -10998,7 +11001,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B65">
         <v>503.75</v>
@@ -11010,7 +11013,7 @@
         <v>66.852976843372602</v>
       </c>
       <c r="F65" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G65">
         <v>667.2</v>
@@ -11024,7 +11027,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B66">
         <v>729.82500000000005</v>
@@ -11036,7 +11039,7 @@
         <v>95.696873860469594</v>
       </c>
       <c r="F66" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G66">
         <v>674.42499999999995</v>
@@ -11050,7 +11053,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B67">
         <v>644.27499999999998</v>
@@ -11062,7 +11065,7 @@
         <v>72.837010703385673</v>
       </c>
       <c r="F67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G67">
         <v>643.57500000000005</v>
@@ -11076,7 +11079,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B68">
         <v>718.97500000000002</v>
@@ -11088,7 +11091,7 @@
         <v>105.3306119820485</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G68">
         <v>673.1</v>
@@ -11102,7 +11105,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B69">
         <v>761.95</v>
@@ -11114,7 +11117,7 @@
         <v>113.16970465315359</v>
       </c>
       <c r="F69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G69">
         <v>695.625</v>
@@ -11128,7 +11131,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B70">
         <v>626.17499999999995</v>
@@ -11140,7 +11143,7 @@
         <v>65.487085240781198</v>
       </c>
       <c r="F70" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G70">
         <v>707.3</v>
@@ -11154,27 +11157,27 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" t="s">
         <v>8</v>
       </c>
-      <c r="D75" t="s">
-        <v>9</v>
-      </c>
-      <c r="G75" t="s">
-        <v>11</v>
-      </c>
       <c r="H75" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I75" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B76">
         <v>10</v>
@@ -11186,7 +11189,7 @@
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G76">
         <v>10</v>
@@ -11200,7 +11203,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>20</v>
@@ -11212,7 +11215,7 @@
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G77">
         <v>20</v>
@@ -11226,7 +11229,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B78">
         <v>30</v>
@@ -11238,7 +11241,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G78">
         <v>30</v>
@@ -11252,7 +11255,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B79">
         <v>40</v>
@@ -11264,7 +11267,7 @@
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G79">
         <v>40</v>
@@ -11278,7 +11281,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B80">
         <v>50</v>
@@ -11290,7 +11293,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G80">
         <v>50</v>
@@ -11304,7 +11307,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B81">
         <v>60</v>
@@ -11316,7 +11319,7 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G81">
         <v>60</v>
@@ -11330,7 +11333,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B82">
         <v>70</v>
@@ -11342,7 +11345,7 @@
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G82">
         <v>70</v>
@@ -11356,7 +11359,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B83">
         <v>80</v>
@@ -11368,7 +11371,7 @@
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G83">
         <v>80</v>
@@ -11382,7 +11385,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B84">
         <v>90</v>
@@ -11394,7 +11397,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G84">
         <v>90</v>
@@ -11408,7 +11411,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B85">
         <v>100</v>
@@ -11420,7 +11423,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G85">
         <v>100</v>
@@ -11434,7 +11437,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B86">
         <v>110</v>
@@ -11446,7 +11449,7 @@
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G86">
         <v>106.55</v>
@@ -11460,7 +11463,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B87">
         <v>120</v>
@@ -11472,7 +11475,7 @@
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G87">
         <v>118.5</v>
@@ -11486,7 +11489,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B88">
         <v>130</v>
@@ -11498,7 +11501,7 @@
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G88">
         <v>126.8</v>
@@ -11512,7 +11515,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B89">
         <v>140</v>
@@ -11524,7 +11527,7 @@
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G89">
         <v>136</v>
@@ -11538,7 +11541,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B90">
         <v>150</v>
@@ -11550,7 +11553,7 @@
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G90">
         <v>147.125</v>
@@ -11564,7 +11567,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B91">
         <v>159.94999999999999</v>
@@ -11576,7 +11579,7 @@
         <v>0.316227766016838</v>
       </c>
       <c r="F91" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G91">
         <v>151.02500000000001</v>
@@ -11590,7 +11593,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B92">
         <v>170</v>
@@ -11602,7 +11605,7 @@
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G92">
         <v>168.35</v>
@@ -11616,7 +11619,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B93">
         <v>180</v>
@@ -11628,7 +11631,7 @@
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G93">
         <v>174.15</v>
@@ -11642,7 +11645,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B94">
         <v>190</v>
@@ -11654,7 +11657,7 @@
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G94">
         <v>185.57499999999999</v>
@@ -11668,7 +11671,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B95">
         <v>200</v>
@@ -11680,7 +11683,7 @@
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G95">
         <v>189.8</v>
@@ -11694,6 +11697,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update mediciones.py y xlsx
</commit_message>
<xml_diff>
--- a/memoria/pasillo/pasillo.xlsx
+++ b/memoria/pasillo/pasillo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diazu\MT-MARL\memoria\pasillo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BA2C38-2077-4AA0-AFFF-EE09AA3F2C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC5007-D1CF-4D73-A08A-D4B193CCCF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77BDEF68-C8AA-4190-91B4-454775195A81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28155" windowHeight="15450" xr2:uid="{77BDEF68-C8AA-4190-91B4-454775195A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="31">
   <si>
     <t>valores_ideales</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>makespan</t>
-  </si>
-  <si>
-    <t>completion_time</t>
   </si>
   <si>
     <t>tiempo_en_acabar</t>
@@ -9266,7 +9263,7 @@
   <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9291,7 +9288,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -10617,7 +10614,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -10626,7 +10623,7 @@
         <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H50" t="s">
         <v>6</v>

</xml_diff>